<commit_message>
Fix #12 - Remove "1-" from Excel tabs
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,20 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="1-Data" sheetId="1" r:id="rId1"/>
-    <sheet name="1-Error Frequency" sheetId="2" r:id="rId2"/>
-    <sheet name="1-Error Count" sheetId="3" r:id="rId3"/>
-    <sheet name="1-Histogram" sheetId="5" r:id="rId4"/>
-    <sheet name="1-Rules" sheetId="4" r:id="rId5"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Error Frequency" sheetId="2" r:id="rId2"/>
+    <sheet name="Error Count" sheetId="3" r:id="rId3"/>
+    <sheet name="Histogram" sheetId="5" r:id="rId4"/>
+    <sheet name="Rules" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="errors_warnings">'1-Data'!$A$133:$A$137</definedName>
-    <definedName name="no_errors_warnings">'1-Data'!$B$133:$B$137</definedName>
-    <definedName name="Series1">'1-Data'!$B$144:$B$146</definedName>
-    <definedName name="with_labels">'1-Data'!$A$144:$A$146</definedName>
+    <definedName name="errors_warnings">Data!$A$133:$A$137</definedName>
+    <definedName name="no_errors_warnings">Data!$B$133:$B$137</definedName>
+    <definedName name="Series1">Data!$B$144:$B$146</definedName>
+    <definedName name="with_labels">Data!$A$144:$A$146</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -611,7 +611,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1-Data'!$A$133</c:f>
+              <c:f>Data!$A$133</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -651,7 +651,7 @@
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'1-Data'!$A$133:$A$137</c:f>
+              <c:f>Data!$A$133:$A$137</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -675,7 +675,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1-Data'!$A$136</c:f>
+              <c:f>Data!$A$136</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1558,7 +1558,7 @@
           </c:dPt>
           <c:cat>
             <c:numRef>
-              <c:f>'1-Error Frequency'!$A$2:$A$15</c:f>
+              <c:f>'Error Frequency'!$A$2:$A$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1567,7 +1567,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1-Error Frequency'!$B$2:$B$15</c:f>
+              <c:f>'Error Frequency'!$B$2:$B$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="14"/>
@@ -1934,7 +1934,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1-Error Count'!$A$2:$A$56</c:f>
+              <c:f>'Error Count'!$A$2:$A$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="55"/>
@@ -1943,7 +1943,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1-Error Count'!$B$2:$B$56</c:f>
+              <c:f>'Error Count'!$B$2:$B$56</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="55"/>
@@ -2227,7 +2227,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1-Error Count'!$D$2:$D$52</c:f>
+              <c:f>'Error Count'!$D$2:$D$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2236,7 +2236,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1-Error Count'!$E$2:$E$52</c:f>
+              <c:f>'Error Count'!$E$2:$E$52</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="51"/>
@@ -2481,7 +2481,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1-Histogram'!$A$2:$A$9</c:f>
+              <c:f>Histogram!$A$2:$A$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2490,7 +2490,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1-Histogram'!$B$2:$B$9</c:f>
+              <c:f>Histogram!$B$2:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2671,7 +2671,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'1-Histogram'!$A$14:$A$21</c:f>
+              <c:f>Histogram!$A$14:$A$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -2680,7 +2680,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'1-Histogram'!$B$14:$B$21</c:f>
+              <c:f>Histogram!$B$14:$B$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
@@ -6411,7 +6411,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A100:C146"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
@@ -6783,7 +6783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix #13 - Create "Summary" tab in Excel and move graphs/summary stats from "1-Data" tab
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,20 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1-Data" sheetId="1" r:id="rId1"/>
-    <sheet name="1-Error Frequency" sheetId="2" r:id="rId2"/>
-    <sheet name="1-Error Count" sheetId="3" r:id="rId3"/>
-    <sheet name="1-Histogram" sheetId="5" r:id="rId4"/>
-    <sheet name="1-Rules" sheetId="4" r:id="rId5"/>
+    <sheet name="Summary" sheetId="6" r:id="rId2"/>
+    <sheet name="1-Error Frequency" sheetId="2" r:id="rId3"/>
+    <sheet name="1-Error Count" sheetId="3" r:id="rId4"/>
+    <sheet name="1-Histogram" sheetId="5" r:id="rId5"/>
+    <sheet name="1-Rules" sheetId="4" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="errors_warnings">'1-Data'!$A$133:$A$137</definedName>
-    <definedName name="no_errors_warnings">'1-Data'!$B$133:$B$137</definedName>
-    <definedName name="Series1">'1-Data'!$B$144:$B$146</definedName>
-    <definedName name="with_labels">'1-Data'!$A$144:$A$146</definedName>
+    <definedName name="errors_warnings">Summary!$A$1:$A$5</definedName>
+    <definedName name="no_errors_warnings">Summary!$B$1:$B$5</definedName>
+    <definedName name="Series1">Summary!$B$12:$B$14</definedName>
+    <definedName name="with_labels">Summary!$A$12:$A$14</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -611,7 +612,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1-Data'!$A$133</c:f>
+              <c:f>Summary!$A$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -645,13 +646,13 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000008-E611-4433-B716-51FD7B591062}"/>
+                <c16:uniqueId val="{00000001-E09E-4196-8B30-6099F297BEFA}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
           <c:val>
             <c:numRef>
-              <c:f>'1-Data'!$A$133:$A$137</c:f>
+              <c:f>Summary!$A$1:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -666,7 +667,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-E611-4433-B716-51FD7B591062}"/>
+              <c16:uniqueId val="{00000002-E09E-4196-8B30-6099F297BEFA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -675,7 +676,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'1-Data'!$A$136</c:f>
+              <c:f>Summary!$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -709,7 +710,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000010-E611-4433-B716-51FD7B591062}"/>
+                <c16:uniqueId val="{00000004-E09E-4196-8B30-6099F297BEFA}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -728,7 +729,7 @@
             </c:spPr>
             <c:extLst>
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{0000000C-E611-4433-B716-51FD7B591062}"/>
+                <c16:uniqueId val="{00000006-E09E-4196-8B30-6099F297BEFA}"/>
               </c:ext>
             </c:extLst>
           </c:dPt>
@@ -749,7 +750,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-E611-4433-B716-51FD7B591062}"/>
+              <c16:uniqueId val="{00000007-E09E-4196-8B30-6099F297BEFA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -780,7 +781,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-E611-4433-B716-51FD7B591062}"/>
+              <c16:uniqueId val="{00000008-E09E-4196-8B30-6099F297BEFA}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1136,7 +1137,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-EEDC-450E-AF17-C9B2343C5A08}"/>
+              <c16:uniqueId val="{00000000-5586-4E97-89FC-683305130B43}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -5516,27 +5517,29 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>281268</xdr:colOff>
-      <xdr:row>113</xdr:row>
-      <xdr:rowOff>27456</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1093134</xdr:colOff>
-      <xdr:row>130</xdr:row>
-      <xdr:rowOff>160806</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>528357</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82B0A3CC-85DE-4B75-A494-1839DA21B21B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -5552,23 +5555,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>257735</xdr:colOff>
-      <xdr:row>139</xdr:row>
-      <xdr:rowOff>179294</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>569258</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>123263</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1900515</xdr:colOff>
-      <xdr:row>155</xdr:row>
-      <xdr:rowOff>160244</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>578221</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104213</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6451BB38-FE46-4867-818D-E61CC19441D5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{337197CE-2428-41A4-BFE4-FE4369684302}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6409,10 +6412,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A100:C146"/>
+  <dimension ref="A100:C130"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="A133" sqref="A133:B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6548,45 +6551,103 @@
       <c r="A130" s="4"/>
       <c r="B130" s="4"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A5B39E-847A-4CAC-A482-820BDFA52C28}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3"/>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B90"/>
   <sheetViews>
@@ -6619,7 +6680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
@@ -6668,7 +6729,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B23"/>
   <sheetViews>
@@ -6779,11 +6840,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fix #6 - Retrieve rule list dynamically from gtfs-rt-validator library
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23010" windowHeight="8940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -35,321 +35,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="110">
-  <si>
-    <t>E045</t>
-  </si>
-  <si>
-    <t>E038</t>
-  </si>
-  <si>
-    <t>W009</t>
-  </si>
-  <si>
-    <t>E011</t>
-  </si>
-  <si>
-    <t>W007</t>
-  </si>
-  <si>
-    <t>W008</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="6">
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>E001</t>
-  </si>
-  <si>
-    <t>Not in POSIX time</t>
-  </si>
-  <si>
-    <t>E002</t>
-  </si>
-  <si>
-    <t>E003</t>
-  </si>
-  <si>
-    <t>E004</t>
-  </si>
-  <si>
-    <t>E006</t>
-  </si>
-  <si>
-    <t>E009</t>
-  </si>
-  <si>
-    <t>E010</t>
-  </si>
-  <si>
-    <t>E012</t>
-  </si>
-  <si>
-    <t>E013</t>
-  </si>
-  <si>
-    <t>E015</t>
-  </si>
-  <si>
-    <t>E016</t>
-  </si>
-  <si>
-    <t>E017</t>
-  </si>
-  <si>
-    <t>E018</t>
-  </si>
-  <si>
-    <t>E019</t>
-  </si>
-  <si>
-    <t>E020</t>
-  </si>
-  <si>
-    <t>E021</t>
-  </si>
-  <si>
-    <t>E022</t>
-  </si>
-  <si>
-    <t>E023</t>
-  </si>
-  <si>
-    <t>E024</t>
-  </si>
-  <si>
-    <t>E025</t>
-  </si>
-  <si>
-    <t>E026</t>
-  </si>
-  <si>
-    <t>E027</t>
-  </si>
-  <si>
-    <t>E028</t>
-  </si>
-  <si>
-    <t>E029</t>
-  </si>
-  <si>
-    <t>E030</t>
-  </si>
-  <si>
-    <t>E031</t>
-  </si>
-  <si>
-    <t>E032</t>
-  </si>
-  <si>
-    <t>E033</t>
-  </si>
-  <si>
-    <t>E034</t>
-  </si>
-  <si>
-    <t>E035</t>
-  </si>
-  <si>
-    <t>E036</t>
-  </si>
-  <si>
-    <t>E037</t>
-  </si>
-  <si>
-    <t>E039</t>
-  </si>
-  <si>
-    <t>E040</t>
-  </si>
-  <si>
-    <t>E041</t>
-  </si>
-  <si>
-    <t>E042</t>
-  </si>
-  <si>
-    <t>E043</t>
-  </si>
-  <si>
-    <t>E044</t>
-  </si>
-  <si>
-    <t>E046</t>
-  </si>
-  <si>
-    <t>E047</t>
-  </si>
-  <si>
-    <t>W001</t>
-  </si>
-  <si>
-    <t>W002</t>
-  </si>
-  <si>
-    <t>W003</t>
-  </si>
-  <si>
-    <t>ID in one feed missing from the other</t>
-  </si>
-  <si>
-    <t>W004</t>
-  </si>
-  <si>
-    <t>W005</t>
-  </si>
-  <si>
-    <t>W006</t>
-  </si>
-  <si>
-    <t>Refresh interval is more than 35 seconds</t>
-  </si>
-  <si>
-    <t>Unsorted stop_sequence</t>
-  </si>
-  <si>
-    <t>GTFS-rt trip_id does not exist in GTFS data</t>
-  </si>
-  <si>
-    <t>GTFS-rt route_id does not exist in GTFS data</t>
-  </si>
-  <si>
-    <t>Missing required trip field for frequency-based exact_times = 0</t>
-  </si>
-  <si>
-    <t>GTFS-rt stop_sequence isn't provided for trip that visits same stop_id more than once</t>
-  </si>
-  <si>
-    <t>location_type not 0 in stops.txt (Note that this is implemented but not executed because it's specific to GTFS - see issue #126)</t>
-  </si>
-  <si>
-    <t>GTFS-rt stop_id does not exist in GTFS data</t>
-  </si>
-  <si>
-    <t>Header timestamp should be greater than or equal to all other timestamps</t>
-  </si>
-  <si>
-    <t>Frequency type 0 trip schedule_relationship should be UNSCHEDULED or empty</t>
-  </si>
-  <si>
-    <t>All stop_ids referenced in GTFS-rt feeds must have the location_type = 0</t>
-  </si>
-  <si>
-    <t>trip_ids with schedule_relationship ADDED must not be in GTFS data</t>
-  </si>
-  <si>
-    <t>GTFS-rt content changed but has the same header timestamp</t>
-  </si>
-  <si>
-    <t>GTFS-rt header timestamp decreased between two sequential iterations</t>
-  </si>
-  <si>
-    <t>GTFS-rt frequency type 1 trip start_time must be a multiple of GTFS headway_secs later than GTFS start_time</t>
-  </si>
-  <si>
-    <t>Invalid start_time format</t>
-  </si>
-  <si>
-    <t>Invalid start_date format</t>
-  </si>
-  <si>
-    <t>Sequential stop_time_update times are not increasing</t>
-  </si>
-  <si>
-    <t>trip start_time does not match first GTFS arrival_time</t>
-  </si>
-  <si>
-    <t>trip direction_id does not match GTFS data</t>
-  </si>
-  <si>
-    <t>stop_time_update departure time is before arrival time</t>
-  </si>
-  <si>
-    <t>Invalid vehicle position</t>
-  </si>
-  <si>
-    <t>Invalid vehicle bearing</t>
-  </si>
-  <si>
-    <t>Vehicle position outside agency coverage area</t>
-  </si>
-  <si>
-    <t>Vehicle position far from trip shape</t>
-  </si>
-  <si>
-    <t>GTFS-rt alert trip_id does not belong to GTFS-rt alert route_id in GTFS trips.txt</t>
-  </si>
-  <si>
-    <t>Alert informed_entity.route_id does not match informed_entity.trip.route_id</t>
-  </si>
-  <si>
-    <t>Alert does not have an informed_entity</t>
-  </si>
-  <si>
-    <t>Alert informed_entity does not have any specifiers</t>
-  </si>
-  <si>
-    <t>GTFS-rt agency_id does not exist in GTFS data</t>
-  </si>
-  <si>
-    <t>GTFS-rt trip.trip_id does not belong to GTFS-rt trip.route_id in GTFS trips.txt</t>
-  </si>
-  <si>
-    <t>Sequential stop_time_updates have the same stop_sequence</t>
-  </si>
-  <si>
-    <t>Sequential stop_time_updates have the same stop_id</t>
-  </si>
-  <si>
-    <t>Invalid header.gtfs_realtime_version</t>
-  </si>
-  <si>
-    <t>FULL_DATASET feeds should not include entity.is_deleted</t>
-  </si>
-  <si>
-    <t>stop_time_update doesn't contain stop_id or stop_sequence</t>
-  </si>
-  <si>
-    <t>trip doesn't have any stop_time_updates</t>
-  </si>
-  <si>
-    <t>arrival or departure provided for NO_DATA stop_time_update</t>
-  </si>
-  <si>
-    <t>stop_time_update doesn't have arrival or departure</t>
-  </si>
-  <si>
-    <t>stop_time_update arrival/departure doesn't have delay or time</t>
-  </si>
-  <si>
-    <t>GTFS-rt stop_time_update stop_sequence and stop_id do not match GTFS</t>
-  </si>
-  <si>
-    <t>GTFS-rt stop_time_update without time doesn't have arrival/departure time in GTFS</t>
-  </si>
-  <si>
-    <t>VehiclePosition and TripUpdate ID pairing mismatch</t>
-  </si>
-  <si>
-    <t>timestamps not populated</t>
-  </si>
-  <si>
-    <t>vehicle_id not populated</t>
-  </si>
-  <si>
-    <t>vehicle speed is unrealistic</t>
-  </si>
-  <si>
-    <t>Missing vehicle_id in trip_update for frequency-based exact_times = 0</t>
-  </si>
-  <si>
-    <t>trip_update missing trip_id</t>
-  </si>
-  <si>
-    <t>Header timestamp is older than 65 seconds</t>
-  </si>
-  <si>
-    <t>schedule_relationship not populated</t>
   </si>
   <si>
     <t>Feeds with errors</t>
@@ -6414,9 +6102,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A100:C130"/>
   <sheetViews>
-    <sheetView topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132:B146"/>
-    </sheetView>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -6560,7 +6246,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A292C7BF-6F8D-412C-B2EF-159C6A625AD5}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
@@ -6576,10 +6262,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>108</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -6592,10 +6278,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>109</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -6628,19 +6314,19 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>107</v>
+        <v>3</v>
       </c>
       <c r="B13" s="3"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>105</v>
+        <v>1</v>
       </c>
       <c r="B14" s="3"/>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>106</v>
+        <v>2</v>
       </c>
       <c r="B15" s="3"/>
     </row>
@@ -6687,8 +6373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6707,7 +6393,7 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D54" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E54">
         <f>SUM(E2:E52)</f>
@@ -6716,7 +6402,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B58">
         <f>SUM(B2:B56)</f>
@@ -6737,7 +6423,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6784,7 +6470,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B11" s="7">
         <f>SUM(B2:B9)</f>
@@ -6830,7 +6516,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B23" s="7">
         <f>SUM(B14:B21)</f>
@@ -6845,413 +6531,14 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T26" sqref="T26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>8</v>
-      </c>
-      <c r="L1" t="s">
-        <v>48</v>
-      </c>
-      <c r="M1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>56</v>
-      </c>
-      <c r="L2" t="s">
-        <v>49</v>
-      </c>
-      <c r="M2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>58</v>
-      </c>
-      <c r="L4" t="s">
-        <v>52</v>
-      </c>
-      <c r="M4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="L5" t="s">
-        <v>53</v>
-      </c>
-      <c r="M5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" t="s">
-        <v>54</v>
-      </c>
-      <c r="M6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" t="s">
-        <v>4</v>
-      </c>
-      <c r="M7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-      <c r="M8" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="L9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B19" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>28</v>
-      </c>
-      <c r="B22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>29</v>
-      </c>
-      <c r="B23" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>30</v>
-      </c>
-      <c r="B24" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B27" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B28" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>35</v>
-      </c>
-      <c r="B29" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>36</v>
-      </c>
-      <c r="B30" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B31" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>38</v>
-      </c>
-      <c r="B32" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>39</v>
-      </c>
-      <c r="B33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>42</v>
-      </c>
-      <c r="B37" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>43</v>
-      </c>
-      <c r="B38" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>44</v>
-      </c>
-      <c r="B39" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>45</v>
-      </c>
-      <c r="B40" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>47</v>
-      </c>
-      <c r="B43" t="s">
-        <v>97</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>